<commit_message>
Added a bunch of graphs
</commit_message>
<xml_diff>
--- a/NANCounts.xlsx
+++ b/NANCounts.xlsx
@@ -196,12 +196,12 @@
     <t>ZWE_Zimbabwe</t>
   </si>
   <si>
+    <t>PAN_Panama</t>
+  </si>
+  <si>
     <t>IRN_Iran (Islamic Republic of)</t>
   </si>
   <si>
-    <t>PAN_Panama</t>
-  </si>
-  <si>
     <t>ZMB_Zambia</t>
   </si>
   <si>
@@ -211,12 +211,12 @@
     <t>HND_Honduras</t>
   </si>
   <si>
+    <t>NIC_Nicaragua</t>
+  </si>
+  <si>
     <t>IDN_Indonesia</t>
   </si>
   <si>
-    <t>NIC_Nicaragua</t>
-  </si>
-  <si>
     <t>BFA_Burkina Faso</t>
   </si>
   <si>
@@ -289,46 +289,49 @@
     <t>SLE_Sierra Leone</t>
   </si>
   <si>
+    <t>UGA_Uganda</t>
+  </si>
+  <si>
+    <t>PAK_Pakistan</t>
+  </si>
+  <si>
+    <t>COD_D.R. of the Congo</t>
+  </si>
+  <si>
+    <t>SLV_El Salvador</t>
+  </si>
+  <si>
+    <t>IRQ_Iraq</t>
+  </si>
+  <si>
+    <t>KWT_Kuwait</t>
+  </si>
+  <si>
     <t>POL_Poland</t>
   </si>
   <si>
+    <t>QAT_Qatar</t>
+  </si>
+  <si>
+    <t>AGO_Angola</t>
+  </si>
+  <si>
+    <t>HUN_Hungary</t>
+  </si>
+  <si>
+    <t>BHR_Bahrain</t>
+  </si>
+  <si>
     <t>SDN_Sudan</t>
   </si>
   <si>
-    <t>BHR_Bahrain</t>
-  </si>
-  <si>
-    <t>HUN_Hungary</t>
-  </si>
-  <si>
     <t>BGR_Bulgaria</t>
   </si>
   <si>
     <t>SAU_Saudi Arabia</t>
   </si>
   <si>
-    <t>IRQ_Iraq</t>
-  </si>
-  <si>
-    <t>QAT_Qatar</t>
-  </si>
-  <si>
-    <t>AGO_Angola</t>
-  </si>
-  <si>
-    <t>KWT_Kuwait</t>
-  </si>
-  <si>
-    <t>PAK_Pakistan</t>
-  </si>
-  <si>
-    <t>UGA_Uganda</t>
-  </si>
-  <si>
-    <t>SLV_El Salvador</t>
-  </si>
-  <si>
-    <t>COD_D.R. of the Congo</t>
+    <t>ETH_Ethiopia</t>
   </si>
   <si>
     <t>MNG_Mongolia</t>
@@ -337,15 +340,12 @@
     <t>MAC_China, Macao SAR</t>
   </si>
   <si>
+    <t>LAO_Lao People's DR</t>
+  </si>
+  <si>
     <t>SWZ_Eswatini</t>
   </si>
   <si>
-    <t>LAO_Lao People's DR</t>
-  </si>
-  <si>
-    <t>ETH_Ethiopia</t>
-  </si>
-  <si>
     <t>MWI_Malawi</t>
   </si>
   <si>
@@ -355,28 +355,28 @@
     <t>BGD_Bangladesh</t>
   </si>
   <si>
+    <t>DZA_Algeria</t>
+  </si>
+  <si>
+    <t>MDG_Madagascar</t>
+  </si>
+  <si>
     <t>NPL_Nepal</t>
   </si>
   <si>
+    <t>HTI_Haiti</t>
+  </si>
+  <si>
+    <t>MLI_Mali</t>
+  </si>
+  <si>
+    <t>GMB_Gambia</t>
+  </si>
+  <si>
     <t>SYR_Syrian Arab Republic</t>
   </si>
   <si>
-    <t>GMB_Gambia</t>
-  </si>
-  <si>
     <t>COG_Congo</t>
-  </si>
-  <si>
-    <t>MLI_Mali</t>
-  </si>
-  <si>
-    <t>HTI_Haiti</t>
-  </si>
-  <si>
-    <t>MDG_Madagascar</t>
-  </si>
-  <si>
-    <t>DZA_Algeria</t>
   </si>
   <si>
     <t>MMR_Myanmar</t>
@@ -945,7 +945,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -953,7 +953,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -961,7 +961,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -969,7 +969,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -977,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -985,7 +985,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -993,7 +993,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1001,7 +1001,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1009,7 +1009,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1017,7 +1017,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1025,7 +1025,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1033,7 +1033,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1041,7 +1041,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1049,7 +1049,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1057,7 +1057,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1065,7 +1065,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1073,7 +1073,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1081,7 +1081,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1089,7 +1089,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1097,7 +1097,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1105,7 +1105,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1113,7 +1113,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1121,7 +1121,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1129,7 +1129,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1137,7 +1137,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1145,7 +1145,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1153,7 +1153,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1161,7 +1161,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1169,7 +1169,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1177,7 +1177,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1185,7 +1185,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1193,7 +1193,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1201,7 +1201,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1209,7 +1209,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1217,7 +1217,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1225,7 +1225,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1233,7 +1233,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1241,7 +1241,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1249,7 +1249,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1257,7 +1257,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1265,7 +1265,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1273,7 +1273,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1281,7 +1281,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1289,7 +1289,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1297,7 +1297,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1305,7 +1305,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1313,7 +1313,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>102</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1321,7 +1321,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1329,7 +1329,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1337,7 +1337,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1345,7 +1345,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1353,7 +1353,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1361,7 +1361,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>144</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1369,7 +1369,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>144</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1377,7 +1377,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1385,7 +1385,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1393,7 +1393,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1401,7 +1401,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1409,7 +1409,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1417,7 +1417,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>180</v>
+        <v>195</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1425,7 +1425,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>180</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1433,7 +1433,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>180</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1441,7 +1441,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1449,7 +1449,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>246</v>
+        <v>256</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1457,7 +1457,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1465,7 +1465,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>255</v>
+        <v>274</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1473,7 +1473,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1481,7 +1481,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1489,7 +1489,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1497,7 +1497,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1505,7 +1505,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1513,7 +1513,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1521,7 +1521,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1529,7 +1529,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1537,7 +1537,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1545,7 +1545,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1553,7 +1553,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1561,7 +1561,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1569,7 +1569,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1577,7 +1577,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1585,7 +1585,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1593,7 +1593,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>348</v>
+        <v>368</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1601,7 +1601,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>354</v>
+        <v>373</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1609,7 +1609,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>366</v>
+        <v>386</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1617,7 +1617,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>366</v>
+        <v>386</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1625,7 +1625,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>366</v>
+        <v>386</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1633,7 +1633,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>366</v>
+        <v>386</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1641,7 +1641,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>366</v>
+        <v>386</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1649,7 +1649,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>378</v>
+        <v>399</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1657,7 +1657,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>450</v>
+        <v>474</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1665,7 +1665,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>450</v>
+        <v>474</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1673,7 +1673,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>450</v>
+        <v>474</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1681,7 +1681,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>450</v>
+        <v>474</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1689,7 +1689,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>450</v>
+        <v>480</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1697,7 +1697,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>450</v>
+        <v>480</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1705,7 +1705,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>450</v>
+        <v>480</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1713,7 +1713,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>450</v>
+        <v>480</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1721,7 +1721,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>450</v>
+        <v>480</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1729,7 +1729,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>450</v>
+        <v>480</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1737,7 +1737,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>464</v>
+        <v>480</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1745,7 +1745,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>464</v>
+        <v>480</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1753,7 +1753,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>464</v>
+        <v>480</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1761,7 +1761,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>464</v>
+        <v>480</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1769,7 +1769,7 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>486</v>
+        <v>504</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1777,7 +1777,7 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>486</v>
+        <v>516</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1785,7 +1785,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>486</v>
+        <v>516</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1793,7 +1793,7 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>486</v>
+        <v>516</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1801,7 +1801,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>494</v>
+        <v>516</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1809,7 +1809,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>512</v>
+        <v>526</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1817,7 +1817,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>524</v>
+        <v>539</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1825,7 +1825,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>572</v>
+        <v>591</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1833,7 +1833,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>584</v>
+        <v>604</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1841,7 +1841,7 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>584</v>
+        <v>604</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1849,7 +1849,7 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>584</v>
+        <v>604</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1857,7 +1857,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>584</v>
+        <v>604</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1865,7 +1865,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>584</v>
+        <v>604</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1873,7 +1873,7 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>584</v>
+        <v>604</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1881,7 +1881,7 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>584</v>
+        <v>604</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1889,7 +1889,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>584</v>
+        <v>604</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1897,7 +1897,7 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>608</v>
+        <v>630</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1905,7 +1905,7 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>632</v>
+        <v>656</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1913,7 +1913,7 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>704</v>
+        <v>734</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1921,7 +1921,7 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>704</v>
+        <v>734</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1929,7 +1929,7 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>704</v>
+        <v>734</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1937,7 +1937,7 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>704</v>
+        <v>734</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1945,7 +1945,7 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>704</v>
+        <v>734</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1953,7 +1953,7 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>704</v>
+        <v>734</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1961,7 +1961,7 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>704</v>
+        <v>734</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1969,7 +1969,7 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>704</v>
+        <v>734</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1977,7 +1977,7 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>744</v>
+        <v>763</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1985,7 +1985,7 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>753</v>
+        <v>773</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1993,7 +1993,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>753</v>
+        <v>773</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2001,7 +2001,7 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>753</v>
+        <v>773</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2009,7 +2009,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>753</v>
+        <v>773</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2017,7 +2017,7 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>753</v>
+        <v>773</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2025,7 +2025,7 @@
         <v>137</v>
       </c>
       <c r="B137">
-        <v>753</v>
+        <v>773</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2033,7 +2033,7 @@
         <v>138</v>
       </c>
       <c r="B138">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2041,7 +2041,7 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2049,7 +2049,7 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2057,7 +2057,7 @@
         <v>141</v>
       </c>
       <c r="B141">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2065,7 +2065,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2073,7 +2073,7 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2081,7 +2081,7 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2089,7 +2089,7 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2097,7 +2097,7 @@
         <v>146</v>
       </c>
       <c r="B146">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2105,7 +2105,7 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2113,7 +2113,7 @@
         <v>148</v>
       </c>
       <c r="B148">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2121,7 +2121,7 @@
         <v>149</v>
       </c>
       <c r="B149">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2129,7 +2129,7 @@
         <v>150</v>
       </c>
       <c r="B150">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2137,7 +2137,7 @@
         <v>151</v>
       </c>
       <c r="B151">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2145,7 +2145,7 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>810</v>
+        <v>860</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2153,7 +2153,7 @@
         <v>153</v>
       </c>
       <c r="B153">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2161,7 +2161,7 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2169,7 +2169,7 @@
         <v>155</v>
       </c>
       <c r="B155">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2177,7 +2177,7 @@
         <v>156</v>
       </c>
       <c r="B156">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2185,7 +2185,7 @@
         <v>157</v>
       </c>
       <c r="B157">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2193,7 +2193,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2201,7 +2201,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2209,7 +2209,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2217,7 +2217,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2225,7 +2225,7 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2233,7 +2233,7 @@
         <v>163</v>
       </c>
       <c r="B163">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2241,7 +2241,7 @@
         <v>164</v>
       </c>
       <c r="B164">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2249,7 +2249,7 @@
         <v>165</v>
       </c>
       <c r="B165">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2257,7 +2257,7 @@
         <v>166</v>
       </c>
       <c r="B166">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2265,7 +2265,7 @@
         <v>167</v>
       </c>
       <c r="B167">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2273,7 +2273,7 @@
         <v>168</v>
       </c>
       <c r="B168">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -2281,7 +2281,7 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2289,7 +2289,7 @@
         <v>170</v>
       </c>
       <c r="B170">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2297,7 +2297,7 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2305,7 +2305,7 @@
         <v>172</v>
       </c>
       <c r="B172">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2313,7 +2313,7 @@
         <v>173</v>
       </c>
       <c r="B173">
-        <v>843</v>
+        <v>873</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2321,7 +2321,7 @@
         <v>174</v>
       </c>
       <c r="B174">
-        <v>932</v>
+        <v>981</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2329,7 +2329,7 @@
         <v>175</v>
       </c>
       <c r="B175">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2337,7 +2337,7 @@
         <v>176</v>
       </c>
       <c r="B176">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2345,7 +2345,7 @@
         <v>177</v>
       </c>
       <c r="B177">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -2353,7 +2353,7 @@
         <v>178</v>
       </c>
       <c r="B178">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2361,7 +2361,7 @@
         <v>179</v>
       </c>
       <c r="B179">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2369,7 +2369,7 @@
         <v>180</v>
       </c>
       <c r="B180">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2377,7 +2377,7 @@
         <v>181</v>
       </c>
       <c r="B181">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2385,7 +2385,7 @@
         <v>182</v>
       </c>
       <c r="B182">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -2393,7 +2393,7 @@
         <v>183</v>
       </c>
       <c r="B183">
-        <v>1158</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2401,7 +2401,7 @@
         <v>184</v>
       </c>
       <c r="B184">
-        <v>1158</v>
+        <v>1223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sent Ken, Jpn, USA data to excel to work on as case studies
</commit_message>
<xml_diff>
--- a/NANCounts.xlsx
+++ b/NANCounts.xlsx
@@ -196,12 +196,12 @@
     <t>ZWE_Zimbabwe</t>
   </si>
   <si>
+    <t>IRN_Iran (Islamic Republic of)</t>
+  </si>
+  <si>
     <t>PAN_Panama</t>
   </si>
   <si>
-    <t>IRN_Iran (Islamic Republic of)</t>
-  </si>
-  <si>
     <t>ZMB_Zambia</t>
   </si>
   <si>
@@ -211,12 +211,12 @@
     <t>HND_Honduras</t>
   </si>
   <si>
+    <t>IDN_Indonesia</t>
+  </si>
+  <si>
     <t>NIC_Nicaragua</t>
   </si>
   <si>
-    <t>IDN_Indonesia</t>
-  </si>
-  <si>
     <t>BFA_Burkina Faso</t>
   </si>
   <si>
@@ -289,63 +289,63 @@
     <t>SLE_Sierra Leone</t>
   </si>
   <si>
+    <t>POL_Poland</t>
+  </si>
+  <si>
+    <t>SDN_Sudan</t>
+  </si>
+  <si>
+    <t>BHR_Bahrain</t>
+  </si>
+  <si>
+    <t>HUN_Hungary</t>
+  </si>
+  <si>
+    <t>BGR_Bulgaria</t>
+  </si>
+  <si>
+    <t>SAU_Saudi Arabia</t>
+  </si>
+  <si>
+    <t>IRQ_Iraq</t>
+  </si>
+  <si>
+    <t>QAT_Qatar</t>
+  </si>
+  <si>
+    <t>AGO_Angola</t>
+  </si>
+  <si>
+    <t>KWT_Kuwait</t>
+  </si>
+  <si>
+    <t>PAK_Pakistan</t>
+  </si>
+  <si>
     <t>UGA_Uganda</t>
   </si>
   <si>
-    <t>PAK_Pakistan</t>
+    <t>SLV_El Salvador</t>
   </si>
   <si>
     <t>COD_D.R. of the Congo</t>
   </si>
   <si>
-    <t>SLV_El Salvador</t>
-  </si>
-  <si>
-    <t>IRQ_Iraq</t>
-  </si>
-  <si>
-    <t>KWT_Kuwait</t>
-  </si>
-  <si>
-    <t>POL_Poland</t>
-  </si>
-  <si>
-    <t>QAT_Qatar</t>
-  </si>
-  <si>
-    <t>AGO_Angola</t>
-  </si>
-  <si>
-    <t>HUN_Hungary</t>
-  </si>
-  <si>
-    <t>BHR_Bahrain</t>
-  </si>
-  <si>
-    <t>SDN_Sudan</t>
-  </si>
-  <si>
-    <t>BGR_Bulgaria</t>
-  </si>
-  <si>
-    <t>SAU_Saudi Arabia</t>
+    <t>MNG_Mongolia</t>
+  </si>
+  <si>
+    <t>MAC_China, Macao SAR</t>
+  </si>
+  <si>
+    <t>SWZ_Eswatini</t>
+  </si>
+  <si>
+    <t>LAO_Lao People's DR</t>
   </si>
   <si>
     <t>ETH_Ethiopia</t>
   </si>
   <si>
-    <t>MNG_Mongolia</t>
-  </si>
-  <si>
-    <t>MAC_China, Macao SAR</t>
-  </si>
-  <si>
-    <t>LAO_Lao People's DR</t>
-  </si>
-  <si>
-    <t>SWZ_Eswatini</t>
-  </si>
-  <si>
     <t>MWI_Malawi</t>
   </si>
   <si>
@@ -355,28 +355,28 @@
     <t>BGD_Bangladesh</t>
   </si>
   <si>
+    <t>NPL_Nepal</t>
+  </si>
+  <si>
+    <t>SYR_Syrian Arab Republic</t>
+  </si>
+  <si>
+    <t>GMB_Gambia</t>
+  </si>
+  <si>
+    <t>COG_Congo</t>
+  </si>
+  <si>
+    <t>MLI_Mali</t>
+  </si>
+  <si>
+    <t>HTI_Haiti</t>
+  </si>
+  <si>
+    <t>MDG_Madagascar</t>
+  </si>
+  <si>
     <t>DZA_Algeria</t>
-  </si>
-  <si>
-    <t>MDG_Madagascar</t>
-  </si>
-  <si>
-    <t>NPL_Nepal</t>
-  </si>
-  <si>
-    <t>HTI_Haiti</t>
-  </si>
-  <si>
-    <t>MLI_Mali</t>
-  </si>
-  <si>
-    <t>GMB_Gambia</t>
-  </si>
-  <si>
-    <t>SYR_Syrian Arab Republic</t>
-  </si>
-  <si>
-    <t>COG_Congo</t>
   </si>
   <si>
     <t>MMR_Myanmar</t>
@@ -945,7 +945,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -953,7 +953,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -961,7 +961,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -969,7 +969,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -977,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -985,7 +985,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -993,7 +993,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1001,7 +1001,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1009,7 +1009,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1017,7 +1017,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1025,7 +1025,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1033,7 +1033,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1041,7 +1041,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1049,7 +1049,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1057,7 +1057,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1065,7 +1065,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1073,7 +1073,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1081,7 +1081,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1089,7 +1089,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1097,7 +1097,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1105,7 +1105,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1113,7 +1113,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1121,7 +1121,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1129,7 +1129,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1137,7 +1137,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1145,7 +1145,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1153,7 +1153,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1161,7 +1161,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1169,7 +1169,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1177,7 +1177,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1185,7 +1185,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1193,7 +1193,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1201,7 +1201,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1209,7 +1209,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1217,7 +1217,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1225,7 +1225,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1233,7 +1233,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1241,7 +1241,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1249,7 +1249,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1257,7 +1257,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1265,7 +1265,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1273,7 +1273,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1281,7 +1281,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1289,7 +1289,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1297,7 +1297,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1305,7 +1305,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1313,7 +1313,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1321,7 +1321,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1329,7 +1329,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1337,7 +1337,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1345,7 +1345,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1353,7 +1353,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1361,7 +1361,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1369,7 +1369,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1377,7 +1377,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1385,7 +1385,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1393,7 +1393,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1401,7 +1401,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1409,7 +1409,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1417,7 +1417,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1425,7 +1425,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1433,7 +1433,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1441,7 +1441,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1449,7 +1449,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1457,7 +1457,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>266</v>
+        <v>246</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1465,7 +1465,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>274</v>
+        <v>255</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1473,7 +1473,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1481,7 +1481,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1489,7 +1489,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1497,7 +1497,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1505,7 +1505,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1513,7 +1513,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1521,7 +1521,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1529,7 +1529,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1537,7 +1537,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1545,7 +1545,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1553,7 +1553,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1561,7 +1561,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1569,7 +1569,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1577,7 +1577,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1585,7 +1585,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1593,7 +1593,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>368</v>
+        <v>348</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1601,7 +1601,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>373</v>
+        <v>354</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1609,7 +1609,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>386</v>
+        <v>366</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1617,7 +1617,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>386</v>
+        <v>366</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1625,7 +1625,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>386</v>
+        <v>366</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1633,7 +1633,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>386</v>
+        <v>366</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1641,7 +1641,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>386</v>
+        <v>366</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1649,7 +1649,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>399</v>
+        <v>378</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1657,7 +1657,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>474</v>
+        <v>450</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1665,7 +1665,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>474</v>
+        <v>450</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1673,7 +1673,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>474</v>
+        <v>450</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1681,7 +1681,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>474</v>
+        <v>450</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1689,7 +1689,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>480</v>
+        <v>450</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1697,7 +1697,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>480</v>
+        <v>450</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1705,7 +1705,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>480</v>
+        <v>450</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1713,7 +1713,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>480</v>
+        <v>450</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1721,7 +1721,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>480</v>
+        <v>450</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1729,7 +1729,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>480</v>
+        <v>450</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1737,7 +1737,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>480</v>
+        <v>464</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1745,7 +1745,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>480</v>
+        <v>464</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1753,7 +1753,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>480</v>
+        <v>464</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1761,7 +1761,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>480</v>
+        <v>464</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1769,7 +1769,7 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>504</v>
+        <v>486</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1777,7 +1777,7 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>516</v>
+        <v>486</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1785,7 +1785,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>516</v>
+        <v>486</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1793,7 +1793,7 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>516</v>
+        <v>486</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1801,7 +1801,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>516</v>
+        <v>494</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1809,7 +1809,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>526</v>
+        <v>512</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1817,7 +1817,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>539</v>
+        <v>524</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1825,7 +1825,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>591</v>
+        <v>572</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1833,7 +1833,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>604</v>
+        <v>584</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1841,7 +1841,7 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>604</v>
+        <v>584</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1849,7 +1849,7 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>604</v>
+        <v>584</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1857,7 +1857,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>604</v>
+        <v>584</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1865,7 +1865,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>604</v>
+        <v>584</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1873,7 +1873,7 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>604</v>
+        <v>584</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1881,7 +1881,7 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>604</v>
+        <v>584</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1889,7 +1889,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>604</v>
+        <v>584</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1897,7 +1897,7 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>630</v>
+        <v>608</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1905,7 +1905,7 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>656</v>
+        <v>632</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1913,7 +1913,7 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>734</v>
+        <v>704</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1921,7 +1921,7 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>734</v>
+        <v>704</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1929,7 +1929,7 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>734</v>
+        <v>704</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1937,7 +1937,7 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>734</v>
+        <v>704</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1945,7 +1945,7 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>734</v>
+        <v>704</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1953,7 +1953,7 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>734</v>
+        <v>704</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1961,7 +1961,7 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>734</v>
+        <v>704</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1969,7 +1969,7 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>734</v>
+        <v>704</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1977,7 +1977,7 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>763</v>
+        <v>744</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1985,7 +1985,7 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>773</v>
+        <v>753</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1993,7 +1993,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>773</v>
+        <v>753</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2001,7 +2001,7 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>773</v>
+        <v>753</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2009,7 +2009,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>773</v>
+        <v>753</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2017,7 +2017,7 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>773</v>
+        <v>753</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2025,7 +2025,7 @@
         <v>137</v>
       </c>
       <c r="B137">
-        <v>773</v>
+        <v>753</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2033,7 +2033,7 @@
         <v>138</v>
       </c>
       <c r="B138">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2041,7 +2041,7 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2049,7 +2049,7 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2057,7 +2057,7 @@
         <v>141</v>
       </c>
       <c r="B141">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2065,7 +2065,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2073,7 +2073,7 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2081,7 +2081,7 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2089,7 +2089,7 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2097,7 +2097,7 @@
         <v>146</v>
       </c>
       <c r="B146">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2105,7 +2105,7 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2113,7 +2113,7 @@
         <v>148</v>
       </c>
       <c r="B148">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2121,7 +2121,7 @@
         <v>149</v>
       </c>
       <c r="B149">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2129,7 +2129,7 @@
         <v>150</v>
       </c>
       <c r="B150">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2137,7 +2137,7 @@
         <v>151</v>
       </c>
       <c r="B151">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2145,7 +2145,7 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2153,7 +2153,7 @@
         <v>153</v>
       </c>
       <c r="B153">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2161,7 +2161,7 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2169,7 +2169,7 @@
         <v>155</v>
       </c>
       <c r="B155">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2177,7 +2177,7 @@
         <v>156</v>
       </c>
       <c r="B156">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2185,7 +2185,7 @@
         <v>157</v>
       </c>
       <c r="B157">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2193,7 +2193,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2201,7 +2201,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2209,7 +2209,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2217,7 +2217,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2225,7 +2225,7 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2233,7 +2233,7 @@
         <v>163</v>
       </c>
       <c r="B163">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2241,7 +2241,7 @@
         <v>164</v>
       </c>
       <c r="B164">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2249,7 +2249,7 @@
         <v>165</v>
       </c>
       <c r="B165">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2257,7 +2257,7 @@
         <v>166</v>
       </c>
       <c r="B166">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2265,7 +2265,7 @@
         <v>167</v>
       </c>
       <c r="B167">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2273,7 +2273,7 @@
         <v>168</v>
       </c>
       <c r="B168">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -2281,7 +2281,7 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2289,7 +2289,7 @@
         <v>170</v>
       </c>
       <c r="B170">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2297,7 +2297,7 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2305,7 +2305,7 @@
         <v>172</v>
       </c>
       <c r="B172">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2313,7 +2313,7 @@
         <v>173</v>
       </c>
       <c r="B173">
-        <v>873</v>
+        <v>843</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2321,7 +2321,7 @@
         <v>174</v>
       </c>
       <c r="B174">
-        <v>981</v>
+        <v>932</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2329,7 +2329,7 @@
         <v>175</v>
       </c>
       <c r="B175">
-        <v>1073</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2337,7 +2337,7 @@
         <v>176</v>
       </c>
       <c r="B176">
-        <v>1073</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2345,7 +2345,7 @@
         <v>177</v>
       </c>
       <c r="B177">
-        <v>1073</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -2353,7 +2353,7 @@
         <v>178</v>
       </c>
       <c r="B178">
-        <v>1073</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2361,7 +2361,7 @@
         <v>179</v>
       </c>
       <c r="B179">
-        <v>1073</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2369,7 +2369,7 @@
         <v>180</v>
       </c>
       <c r="B180">
-        <v>1073</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2377,7 +2377,7 @@
         <v>181</v>
       </c>
       <c r="B181">
-        <v>1073</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2385,7 +2385,7 @@
         <v>182</v>
       </c>
       <c r="B182">
-        <v>1073</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -2393,7 +2393,7 @@
         <v>183</v>
       </c>
       <c r="B183">
-        <v>1223</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2401,7 +2401,7 @@
         <v>184</v>
       </c>
       <c r="B184">
-        <v>1223</v>
+        <v>1158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added per capita gdp data
</commit_message>
<xml_diff>
--- a/NANCounts.xlsx
+++ b/NANCounts.xlsx
@@ -22,144 +22,144 @@
     <t>country</t>
   </si>
   <si>
+    <t>ITA_Italy</t>
+  </si>
+  <si>
+    <t>FIN_Finland</t>
+  </si>
+  <si>
     <t>CAN_Canada</t>
   </si>
   <si>
+    <t>CHE_Switzerland</t>
+  </si>
+  <si>
+    <t>ISR_Israel</t>
+  </si>
+  <si>
+    <t>ISL_Iceland</t>
+  </si>
+  <si>
+    <t>IRL_Ireland</t>
+  </si>
+  <si>
+    <t>IND_India</t>
+  </si>
+  <si>
+    <t>COL_Colombia</t>
+  </si>
+  <si>
+    <t>CRI_Costa Rica</t>
+  </si>
+  <si>
+    <t>GTM_Guatemala</t>
+  </si>
+  <si>
+    <t>THA_Thailand</t>
+  </si>
+  <si>
+    <t>CYP_Cyprus</t>
+  </si>
+  <si>
+    <t>DEU_Germany</t>
+  </si>
+  <si>
+    <t>NOR_Norway</t>
+  </si>
+  <si>
+    <t>SWE_Sweden</t>
+  </si>
+  <si>
+    <t>DNK_Denmark</t>
+  </si>
+  <si>
+    <t>MUS_Mauritius</t>
+  </si>
+  <si>
+    <t>ECU_Ecuador</t>
+  </si>
+  <si>
+    <t>EGY_Egypt</t>
+  </si>
+  <si>
+    <t>ESP_Spain</t>
+  </si>
+  <si>
+    <t>MEX_Mexico</t>
+  </si>
+  <si>
+    <t>GBR_United Kingdom</t>
+  </si>
+  <si>
+    <t>NZL_New Zealand</t>
+  </si>
+  <si>
+    <t>JPN_Japan</t>
+  </si>
+  <si>
+    <t>FRA_France</t>
+  </si>
+  <si>
+    <t>BOL_Bolivia (Plurinational State of)</t>
+  </si>
+  <si>
+    <t>PER_Peru</t>
+  </si>
+  <si>
+    <t>ZAF_South Africa</t>
+  </si>
+  <si>
+    <t>NLD_Netherlands</t>
+  </si>
+  <si>
+    <t>VEN_Venezuela (Bolivarian Republic of)</t>
+  </si>
+  <si>
+    <t>ARG_Argentina</t>
+  </si>
+  <si>
+    <t>USA_United States</t>
+  </si>
+  <si>
+    <t>URY_Uruguay</t>
+  </si>
+  <si>
+    <t>AUS_Australia</t>
+  </si>
+  <si>
+    <t>AUT_Austria</t>
+  </si>
+  <si>
+    <t>PHL_Philippines</t>
+  </si>
+  <si>
+    <t>BEL_Belgium</t>
+  </si>
+  <si>
+    <t>BRA_Brazil</t>
+  </si>
+  <si>
+    <t>LUX_Luxembourg</t>
+  </si>
+  <si>
+    <t>MAR_Morocco</t>
+  </si>
+  <si>
+    <t>PRT_Portugal</t>
+  </si>
+  <si>
+    <t>LKA_Sri Lanka</t>
+  </si>
+  <si>
+    <t>TTO_Trinidad and Tobago</t>
+  </si>
+  <si>
     <t>KEN_Kenya</t>
   </si>
   <si>
-    <t>FRA_France</t>
-  </si>
-  <si>
-    <t>CHE_Switzerland</t>
-  </si>
-  <si>
-    <t>PHL_Philippines</t>
-  </si>
-  <si>
-    <t>JPN_Japan</t>
-  </si>
-  <si>
-    <t>COL_Colombia</t>
-  </si>
-  <si>
-    <t>ITA_Italy</t>
-  </si>
-  <si>
-    <t>ISR_Israel</t>
-  </si>
-  <si>
-    <t>CRI_Costa Rica</t>
-  </si>
-  <si>
-    <t>SWE_Sweden</t>
-  </si>
-  <si>
-    <t>PER_Peru</t>
-  </si>
-  <si>
-    <t>ISL_Iceland</t>
-  </si>
-  <si>
-    <t>DEU_Germany</t>
-  </si>
-  <si>
-    <t>IRL_Ireland</t>
-  </si>
-  <si>
-    <t>IND_India</t>
-  </si>
-  <si>
-    <t>DNK_Denmark</t>
-  </si>
-  <si>
-    <t>PRT_Portugal</t>
-  </si>
-  <si>
-    <t>ECU_Ecuador</t>
-  </si>
-  <si>
-    <t>EGY_Egypt</t>
-  </si>
-  <si>
-    <t>ESP_Spain</t>
-  </si>
-  <si>
-    <t>GTM_Guatemala</t>
-  </si>
-  <si>
-    <t>FIN_Finland</t>
-  </si>
-  <si>
-    <t>CYP_Cyprus</t>
-  </si>
-  <si>
-    <t>THA_Thailand</t>
-  </si>
-  <si>
-    <t>GBR_United Kingdom</t>
-  </si>
-  <si>
-    <t>BRA_Brazil</t>
-  </si>
-  <si>
-    <t>MUS_Mauritius</t>
-  </si>
-  <si>
-    <t>ZAF_South Africa</t>
-  </si>
-  <si>
-    <t>VEN_Venezuela (Bolivarian Republic of)</t>
-  </si>
-  <si>
-    <t>ARG_Argentina</t>
-  </si>
-  <si>
-    <t>USA_United States</t>
-  </si>
-  <si>
-    <t>URY_Uruguay</t>
-  </si>
-  <si>
-    <t>AUS_Australia</t>
-  </si>
-  <si>
-    <t>AUT_Austria</t>
-  </si>
-  <si>
-    <t>MEX_Mexico</t>
-  </si>
-  <si>
-    <t>NLD_Netherlands</t>
-  </si>
-  <si>
-    <t>MAR_Morocco</t>
-  </si>
-  <si>
-    <t>NOR_Norway</t>
-  </si>
-  <si>
-    <t>BEL_Belgium</t>
-  </si>
-  <si>
-    <t>LKA_Sri Lanka</t>
-  </si>
-  <si>
-    <t>BOL_Bolivia (Plurinational State of)</t>
-  </si>
-  <si>
-    <t>NZL_New Zealand</t>
-  </si>
-  <si>
-    <t>TTO_Trinidad and Tobago</t>
-  </si>
-  <si>
     <t>TUR_Turkey</t>
   </si>
   <si>
-    <t>LUX_Luxembourg</t>
-  </si>
-  <si>
     <t>CHL_Chile</t>
   </si>
   <si>
@@ -169,22 +169,25 @@
     <t>PRY_Paraguay</t>
   </si>
   <si>
+    <t>TWN_Taiwan</t>
+  </si>
+  <si>
     <t>DOM_Dominican Republic</t>
   </si>
   <si>
-    <t>TWN_Taiwan</t>
-  </si>
-  <si>
     <t>CHN_China</t>
   </si>
   <si>
+    <t>NGA_Nigeria</t>
+  </si>
+  <si>
     <t>KOR_Republic of Korea</t>
   </si>
   <si>
     <t>JAM_Jamaica</t>
   </si>
   <si>
-    <t>NGA_Nigeria</t>
+    <t>PAN_Panama</t>
   </si>
   <si>
     <t>MLT_Malta</t>
@@ -193,363 +196,363 @@
     <t>JOR_Jordan</t>
   </si>
   <si>
+    <t>HND_Honduras</t>
+  </si>
+  <si>
     <t>ZWE_Zimbabwe</t>
   </si>
   <si>
+    <t>ZMB_Zambia</t>
+  </si>
+  <si>
+    <t>MYS_Malaysia</t>
+  </si>
+  <si>
     <t>IRN_Iran (Islamic Republic of)</t>
   </si>
   <si>
-    <t>PAN_Panama</t>
-  </si>
-  <si>
-    <t>ZMB_Zambia</t>
-  </si>
-  <si>
-    <t>MYS_Malaysia</t>
-  </si>
-  <si>
-    <t>HND_Honduras</t>
+    <t>NIC_Nicaragua</t>
   </si>
   <si>
     <t>IDN_Indonesia</t>
   </si>
   <si>
-    <t>NIC_Nicaragua</t>
-  </si>
-  <si>
     <t>BFA_Burkina Faso</t>
   </si>
   <si>
+    <t>GAB_Gabon</t>
+  </si>
+  <si>
+    <t>TZA_U.R. of Tanzania: Mainland</t>
+  </si>
+  <si>
+    <t>ROU_Romania</t>
+  </si>
+  <si>
+    <t>RWA_Rwanda</t>
+  </si>
+  <si>
+    <t>TUN_Tunisia</t>
+  </si>
+  <si>
+    <t>BRB_Barbados</t>
+  </si>
+  <si>
+    <t>CIV_Côte d'Ivoire</t>
+  </si>
+  <si>
+    <t>CMR_Cameroon</t>
+  </si>
+  <si>
     <t>BWA_Botswana</t>
   </si>
   <si>
-    <t>BRB_Barbados</t>
-  </si>
-  <si>
-    <t>TUN_Tunisia</t>
+    <t>NER_Niger</t>
+  </si>
+  <si>
+    <t>HKG_China, Hong Kong SAR</t>
+  </si>
+  <si>
+    <t>SEN_Senegal</t>
+  </si>
+  <si>
+    <t>NAM_Namibia</t>
   </si>
   <si>
     <t>SGP_Singapore</t>
   </si>
   <si>
-    <t>SEN_Senegal</t>
-  </si>
-  <si>
-    <t>TZA_U.R. of Tanzania: Mainland</t>
-  </si>
-  <si>
-    <t>CIV_Côte d'Ivoire</t>
-  </si>
-  <si>
-    <t>GAB_Gabon</t>
-  </si>
-  <si>
-    <t>NER_Niger</t>
-  </si>
-  <si>
     <t>MOZ_Mozambique</t>
   </si>
   <si>
-    <t>ROU_Romania</t>
-  </si>
-  <si>
-    <t>RWA_Rwanda</t>
-  </si>
-  <si>
-    <t>NAM_Namibia</t>
-  </si>
-  <si>
-    <t>HKG_China, Hong Kong SAR</t>
-  </si>
-  <si>
-    <t>CMR_Cameroon</t>
-  </si>
-  <si>
     <t>MRT_Mauritania</t>
   </si>
   <si>
     <t>BEN_Benin</t>
   </si>
   <si>
+    <t>CAF_Central African Republic</t>
+  </si>
+  <si>
     <t>LSO_Lesotho</t>
   </si>
   <si>
     <t>BDI_Burundi</t>
   </si>
   <si>
-    <t>CAF_Central African Republic</t>
+    <t>FJI_Fiji</t>
   </si>
   <si>
     <t>TGO_Togo</t>
   </si>
   <si>
-    <t>FJI_Fiji</t>
-  </si>
-  <si>
     <t>SLE_Sierra Leone</t>
   </si>
   <si>
+    <t>SLV_El Salvador</t>
+  </si>
+  <si>
+    <t>UGA_Uganda</t>
+  </si>
+  <si>
+    <t>COD_D.R. of the Congo</t>
+  </si>
+  <si>
+    <t>PAK_Pakistan</t>
+  </si>
+  <si>
+    <t>ETH_Ethiopia</t>
+  </si>
+  <si>
+    <t>MWI_Malawi</t>
+  </si>
+  <si>
+    <t>GHA_Ghana</t>
+  </si>
+  <si>
+    <t>QAT_Qatar</t>
+  </si>
+  <si>
+    <t>KWT_Kuwait</t>
+  </si>
+  <si>
+    <t>BHR_Bahrain</t>
+  </si>
+  <si>
+    <t>BGR_Bulgaria</t>
+  </si>
+  <si>
+    <t>SDN_Sudan</t>
+  </si>
+  <si>
     <t>POL_Poland</t>
   </si>
   <si>
-    <t>SDN_Sudan</t>
-  </si>
-  <si>
-    <t>BHR_Bahrain</t>
+    <t>SAU_Saudi Arabia</t>
+  </si>
+  <si>
+    <t>IRQ_Iraq</t>
   </si>
   <si>
     <t>HUN_Hungary</t>
   </si>
   <si>
-    <t>BGR_Bulgaria</t>
-  </si>
-  <si>
-    <t>SAU_Saudi Arabia</t>
-  </si>
-  <si>
-    <t>IRQ_Iraq</t>
-  </si>
-  <si>
-    <t>QAT_Qatar</t>
-  </si>
-  <si>
     <t>AGO_Angola</t>
   </si>
   <si>
-    <t>KWT_Kuwait</t>
-  </si>
-  <si>
-    <t>PAK_Pakistan</t>
-  </si>
-  <si>
-    <t>UGA_Uganda</t>
-  </si>
-  <si>
-    <t>SLV_El Salvador</t>
-  </si>
-  <si>
-    <t>COD_D.R. of the Congo</t>
+    <t>SWZ_Eswatini</t>
+  </si>
+  <si>
+    <t>MAC_China, Macao SAR</t>
+  </si>
+  <si>
+    <t>LAO_Lao People's DR</t>
   </si>
   <si>
     <t>MNG_Mongolia</t>
   </si>
   <si>
-    <t>MAC_China, Macao SAR</t>
-  </si>
-  <si>
-    <t>SWZ_Eswatini</t>
-  </si>
-  <si>
-    <t>LAO_Lao People's DR</t>
-  </si>
-  <si>
-    <t>ETH_Ethiopia</t>
-  </si>
-  <si>
-    <t>MWI_Malawi</t>
-  </si>
-  <si>
-    <t>GHA_Ghana</t>
-  </si>
-  <si>
     <t>BGD_Bangladesh</t>
   </si>
   <si>
     <t>NPL_Nepal</t>
   </si>
   <si>
+    <t>MDG_Madagascar</t>
+  </si>
+  <si>
+    <t>HTI_Haiti</t>
+  </si>
+  <si>
+    <t>COG_Congo</t>
+  </si>
+  <si>
     <t>SYR_Syrian Arab Republic</t>
   </si>
   <si>
     <t>GMB_Gambia</t>
   </si>
   <si>
-    <t>COG_Congo</t>
+    <t>DZA_Algeria</t>
   </si>
   <si>
     <t>MLI_Mali</t>
   </si>
   <si>
-    <t>HTI_Haiti</t>
-  </si>
-  <si>
-    <t>MDG_Madagascar</t>
-  </si>
-  <si>
-    <t>DZA_Algeria</t>
-  </si>
-  <si>
     <t>MMR_Myanmar</t>
   </si>
   <si>
     <t>LBR_Liberia</t>
   </si>
   <si>
+    <t>GIN_Guinea</t>
+  </si>
+  <si>
+    <t>TCD_Chad</t>
+  </si>
+  <si>
+    <t>CPV_Cabo Verde</t>
+  </si>
+  <si>
+    <t>COM_Comoros</t>
+  </si>
+  <si>
+    <t>GNQ_Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>GNB_Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>SYC_Seychelles</t>
+  </si>
+  <si>
     <t>VNM_Viet Nam</t>
   </si>
   <si>
     <t>KHM_Cambodia</t>
   </si>
   <si>
+    <t>BLZ_Belize</t>
+  </si>
+  <si>
+    <t>ALB_Albania</t>
+  </si>
+  <si>
     <t>MDV_Maldives</t>
   </si>
   <si>
+    <t>ARE_United Arab Emirates</t>
+  </si>
+  <si>
+    <t>GUY_Guyana</t>
+  </si>
+  <si>
     <t>BRN_Brunei Darussalam</t>
   </si>
   <si>
-    <t>BLZ_Belize</t>
-  </si>
-  <si>
-    <t>ALB_Albania</t>
-  </si>
-  <si>
-    <t>ARE_United Arab Emirates</t>
-  </si>
-  <si>
-    <t>GUY_Guyana</t>
-  </si>
-  <si>
-    <t>GIN_Guinea</t>
-  </si>
-  <si>
-    <t>GNB_Guinea-Bissau</t>
-  </si>
-  <si>
-    <t>CPV_Cabo Verde</t>
-  </si>
-  <si>
-    <t>TCD_Chad</t>
-  </si>
-  <si>
-    <t>SYC_Seychelles</t>
-  </si>
-  <si>
-    <t>GNQ_Equatorial Guinea</t>
-  </si>
-  <si>
-    <t>COM_Comoros</t>
+    <t>DJI_Djibouti</t>
+  </si>
+  <si>
+    <t>MSR_Montserrat</t>
+  </si>
+  <si>
+    <t>CYM_Cayman Islands</t>
+  </si>
+  <si>
+    <t>TCA_Turks and Caicos Islands</t>
+  </si>
+  <si>
+    <t>BTN_Bhutan</t>
+  </si>
+  <si>
+    <t>OMN_Oman</t>
+  </si>
+  <si>
+    <t>DMA_Dominica</t>
+  </si>
+  <si>
+    <t>BHS_Bahamas</t>
+  </si>
+  <si>
+    <t>ATG_Antigua and Barbuda</t>
+  </si>
+  <si>
+    <t>VCT_St. Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t>VGB_British Virgin Islands</t>
+  </si>
+  <si>
+    <t>AIA_Anguilla</t>
+  </si>
+  <si>
+    <t>BMU_Bermuda</t>
+  </si>
+  <si>
+    <t>SUR_Suriname</t>
+  </si>
+  <si>
+    <t>ABW_Aruba</t>
+  </si>
+  <si>
+    <t>LBN_Lebanon</t>
+  </si>
+  <si>
+    <t>GRD_Grenada</t>
+  </si>
+  <si>
+    <t>LCA_Saint Lucia</t>
+  </si>
+  <si>
+    <t>PSE_State of Palestine</t>
+  </si>
+  <si>
+    <t>STP_Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t>KNA_Saint Kitts and Nevis</t>
+  </si>
+  <si>
+    <t>MDA_Republic of Moldova</t>
+  </si>
+  <si>
+    <t>LVA_Latvia</t>
+  </si>
+  <si>
+    <t>LTU_Lithuania</t>
+  </si>
+  <si>
+    <t>ARM_Armenia</t>
+  </si>
+  <si>
+    <t>UKR_Ukraine</t>
+  </si>
+  <si>
+    <t>TJK_Tajikistan</t>
+  </si>
+  <si>
+    <t>SRB_Serbia</t>
+  </si>
+  <si>
+    <t>KGZ_Kyrgyzstan</t>
   </si>
   <si>
     <t>KAZ_Kazakhstan</t>
   </si>
   <si>
-    <t>MDA_Republic of Moldova</t>
+    <t>SVK_Slovakia</t>
+  </si>
+  <si>
+    <t>HRV_Croatia</t>
+  </si>
+  <si>
+    <t>CZE_Czech Republic</t>
+  </si>
+  <si>
+    <t>RUS_Russian Federation</t>
   </si>
   <si>
     <t>SVN_Slovenia</t>
   </si>
   <si>
-    <t>LVA_Latvia</t>
-  </si>
-  <si>
-    <t>TJK_Tajikistan</t>
-  </si>
-  <si>
-    <t>SRB_Serbia</t>
-  </si>
-  <si>
-    <t>HRV_Croatia</t>
-  </si>
-  <si>
-    <t>LTU_Lithuania</t>
-  </si>
-  <si>
-    <t>CZE_Czech Republic</t>
-  </si>
-  <si>
-    <t>UKR_Ukraine</t>
-  </si>
-  <si>
-    <t>RUS_Russian Federation</t>
-  </si>
-  <si>
-    <t>KGZ_Kyrgyzstan</t>
-  </si>
-  <si>
-    <t>ARM_Armenia</t>
-  </si>
-  <si>
     <t>EST_Estonia</t>
   </si>
   <si>
-    <t>SVK_Slovakia</t>
-  </si>
-  <si>
-    <t>BHS_Bahamas</t>
-  </si>
-  <si>
-    <t>VGB_British Virgin Islands</t>
-  </si>
-  <si>
-    <t>BMU_Bermuda</t>
-  </si>
-  <si>
-    <t>VCT_St. Vincent and the Grenadines</t>
-  </si>
-  <si>
-    <t>BTN_Bhutan</t>
-  </si>
-  <si>
-    <t>ATG_Antigua and Barbuda</t>
-  </si>
-  <si>
-    <t>AIA_Anguilla</t>
-  </si>
-  <si>
-    <t>TCA_Turks and Caicos Islands</t>
-  </si>
-  <si>
-    <t>ABW_Aruba</t>
-  </si>
-  <si>
-    <t>MSR_Montserrat</t>
-  </si>
-  <si>
-    <t>SUR_Suriname</t>
-  </si>
-  <si>
-    <t>STP_Sao Tome and Principe</t>
-  </si>
-  <si>
-    <t>CYM_Cayman Islands</t>
-  </si>
-  <si>
-    <t>DJI_Djibouti</t>
-  </si>
-  <si>
-    <t>LCA_Saint Lucia</t>
-  </si>
-  <si>
-    <t>DMA_Dominica</t>
-  </si>
-  <si>
-    <t>OMN_Oman</t>
-  </si>
-  <si>
-    <t>LBN_Lebanon</t>
-  </si>
-  <si>
-    <t>PSE_State of Palestine</t>
-  </si>
-  <si>
-    <t>GRD_Grenada</t>
-  </si>
-  <si>
-    <t>KNA_Saint Kitts and Nevis</t>
-  </si>
-  <si>
     <t>YEM_Yemen</t>
   </si>
   <si>
+    <t>TKM_Turkmenistan</t>
+  </si>
+  <si>
+    <t>MNE_Montenegro</t>
+  </si>
+  <si>
+    <t>MKD_North Macedonia</t>
+  </si>
+  <si>
     <t>GEO_Georgia</t>
   </si>
   <si>
-    <t>MKD_North Macedonia</t>
-  </si>
-  <si>
-    <t>MNE_Montenegro</t>
-  </si>
-  <si>
     <t>AZE_Azerbaijan</t>
   </si>
   <si>
@@ -559,16 +562,13 @@
     <t>BLR_Belarus</t>
   </si>
   <si>
-    <t>TKM_Turkmenistan</t>
-  </si>
-  <si>
     <t>UZB_Uzbekistan</t>
   </si>
   <si>
+    <t>CUW_Curaçao</t>
+  </si>
+  <si>
     <t>SXM_Sint Maarten (Dutch part)</t>
-  </si>
-  <si>
-    <t>CUW_Curaçao</t>
   </si>
 </sst>
 </file>
@@ -945,7 +945,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -953,7 +953,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -961,7 +961,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -969,7 +969,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -977,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -985,7 +985,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -993,7 +993,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1001,7 +1001,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1009,7 +1009,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1017,7 +1017,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1025,7 +1025,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1033,7 +1033,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1041,7 +1041,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1049,7 +1049,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1057,7 +1057,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1065,7 +1065,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1073,7 +1073,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1081,7 +1081,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1089,7 +1089,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1097,7 +1097,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1105,7 +1105,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1113,7 +1113,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1121,7 +1121,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1129,7 +1129,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1137,7 +1137,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1145,7 +1145,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1153,7 +1153,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1161,7 +1161,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1169,7 +1169,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1177,7 +1177,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1185,7 +1185,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1193,7 +1193,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1201,7 +1201,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1209,7 +1209,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1217,7 +1217,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1225,7 +1225,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1233,7 +1233,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1241,7 +1241,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1249,7 +1249,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1257,7 +1257,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1265,7 +1265,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1273,7 +1273,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1281,7 +1281,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1289,7 +1289,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1297,7 +1297,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1305,7 +1305,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1313,7 +1313,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>102</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1321,7 +1321,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>108</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1329,7 +1329,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>108</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1337,7 +1337,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>108</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1345,7 +1345,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>108</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1353,7 +1353,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>126</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1361,7 +1361,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>144</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1369,7 +1369,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>144</v>
+        <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1377,7 +1377,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>156</v>
+        <v>190</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1385,7 +1385,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>162</v>
+        <v>208</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1393,7 +1393,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>162</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1401,7 +1401,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>162</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1409,7 +1409,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>180</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1417,7 +1417,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>180</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1425,7 +1425,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>180</v>
+        <v>238</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1433,7 +1433,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>180</v>
+        <v>238</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1441,7 +1441,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>186</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1449,7 +1449,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>246</v>
+        <v>274</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1457,7 +1457,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>246</v>
+        <v>334</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1465,7 +1465,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>255</v>
+        <v>337</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1473,7 +1473,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1481,7 +1481,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1489,7 +1489,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1497,7 +1497,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1505,7 +1505,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1513,7 +1513,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1521,7 +1521,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1529,7 +1529,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1537,7 +1537,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1545,7 +1545,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1553,7 +1553,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1561,7 +1561,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1569,7 +1569,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1577,7 +1577,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1585,7 +1585,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1593,7 +1593,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>348</v>
+        <v>436</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1601,7 +1601,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>354</v>
+        <v>436</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1609,7 +1609,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>366</v>
+        <v>454</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1617,7 +1617,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>366</v>
+        <v>454</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1625,7 +1625,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>366</v>
+        <v>454</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1633,7 +1633,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>366</v>
+        <v>454</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1641,7 +1641,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>366</v>
+        <v>454</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1649,7 +1649,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>378</v>
+        <v>472</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1657,7 +1657,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>450</v>
+        <v>492</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1665,7 +1665,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>450</v>
+        <v>492</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1673,7 +1673,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>450</v>
+        <v>492</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1681,7 +1681,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>450</v>
+        <v>492</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1689,7 +1689,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>450</v>
+        <v>522</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1697,7 +1697,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>450</v>
+        <v>564</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1705,7 +1705,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>450</v>
+        <v>582</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1713,7 +1713,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>450</v>
+        <v>598</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1721,7 +1721,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>450</v>
+        <v>598</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1729,7 +1729,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>450</v>
+        <v>598</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1737,7 +1737,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>464</v>
+        <v>598</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1745,7 +1745,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>464</v>
+        <v>598</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1753,7 +1753,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>464</v>
+        <v>598</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1761,7 +1761,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>464</v>
+        <v>598</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1769,7 +1769,7 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>486</v>
+        <v>598</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1777,7 +1777,7 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>486</v>
+        <v>598</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1785,7 +1785,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>486</v>
+        <v>598</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1793,7 +1793,7 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>486</v>
+        <v>634</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1801,7 +1801,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>494</v>
+        <v>634</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1809,7 +1809,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>512</v>
+        <v>634</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1817,7 +1817,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>524</v>
+        <v>634</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1825,7 +1825,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>572</v>
+        <v>654</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1833,7 +1833,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>584</v>
+        <v>672</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1841,7 +1841,7 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>584</v>
+        <v>672</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1849,7 +1849,7 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>584</v>
+        <v>672</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1857,7 +1857,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>584</v>
+        <v>672</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1865,7 +1865,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>584</v>
+        <v>672</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1873,7 +1873,7 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>584</v>
+        <v>672</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1881,7 +1881,7 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>584</v>
+        <v>672</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1889,7 +1889,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>584</v>
+        <v>672</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1897,7 +1897,7 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>608</v>
+        <v>708</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1905,7 +1905,7 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>632</v>
+        <v>744</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1913,7 +1913,7 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>704</v>
+        <v>826</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1921,7 +1921,7 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>704</v>
+        <v>841</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1929,7 +1929,7 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>704</v>
+        <v>841</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1937,7 +1937,7 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>704</v>
+        <v>841</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1945,7 +1945,7 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>704</v>
+        <v>841</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1953,7 +1953,7 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>704</v>
+        <v>841</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1961,7 +1961,7 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>704</v>
+        <v>841</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1969,7 +1969,7 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>704</v>
+        <v>852</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1977,7 +1977,7 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>744</v>
+        <v>852</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1985,7 +1985,7 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>753</v>
+        <v>852</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1993,7 +1993,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>753</v>
+        <v>852</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2001,7 +2001,7 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>753</v>
+        <v>852</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2009,7 +2009,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>753</v>
+        <v>852</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2017,7 +2017,7 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>753</v>
+        <v>852</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2025,7 +2025,7 @@
         <v>137</v>
       </c>
       <c r="B137">
-        <v>753</v>
+        <v>852</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2033,7 +2033,7 @@
         <v>138</v>
       </c>
       <c r="B138">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2041,7 +2041,7 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2049,7 +2049,7 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2057,7 +2057,7 @@
         <v>141</v>
       </c>
       <c r="B141">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2065,7 +2065,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2073,7 +2073,7 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2081,7 +2081,7 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2089,7 +2089,7 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2097,7 +2097,7 @@
         <v>146</v>
       </c>
       <c r="B146">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2105,7 +2105,7 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2113,7 +2113,7 @@
         <v>148</v>
       </c>
       <c r="B148">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2121,7 +2121,7 @@
         <v>149</v>
       </c>
       <c r="B149">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2129,7 +2129,7 @@
         <v>150</v>
       </c>
       <c r="B150">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2137,7 +2137,7 @@
         <v>151</v>
       </c>
       <c r="B151">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2145,7 +2145,7 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>810</v>
+        <v>991</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2153,7 +2153,7 @@
         <v>153</v>
       </c>
       <c r="B153">
-        <v>843</v>
+        <v>991</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2161,7 +2161,7 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>843</v>
+        <v>991</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2169,7 +2169,7 @@
         <v>155</v>
       </c>
       <c r="B155">
-        <v>843</v>
+        <v>991</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2177,7 +2177,7 @@
         <v>156</v>
       </c>
       <c r="B156">
-        <v>843</v>
+        <v>991</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2185,7 +2185,7 @@
         <v>157</v>
       </c>
       <c r="B157">
-        <v>843</v>
+        <v>991</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2193,7 +2193,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>843</v>
+        <v>991</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2201,7 +2201,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2209,7 +2209,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2217,7 +2217,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2225,7 +2225,7 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2233,7 +2233,7 @@
         <v>163</v>
       </c>
       <c r="B163">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2241,7 +2241,7 @@
         <v>164</v>
       </c>
       <c r="B164">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2249,7 +2249,7 @@
         <v>165</v>
       </c>
       <c r="B165">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2257,7 +2257,7 @@
         <v>166</v>
       </c>
       <c r="B166">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2265,7 +2265,7 @@
         <v>167</v>
       </c>
       <c r="B167">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2273,7 +2273,7 @@
         <v>168</v>
       </c>
       <c r="B168">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -2281,7 +2281,7 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2289,7 +2289,7 @@
         <v>170</v>
       </c>
       <c r="B170">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2297,7 +2297,7 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2305,7 +2305,7 @@
         <v>172</v>
       </c>
       <c r="B172">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2313,7 +2313,7 @@
         <v>173</v>
       </c>
       <c r="B173">
-        <v>843</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2321,7 +2321,7 @@
         <v>174</v>
       </c>
       <c r="B174">
-        <v>932</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2329,7 +2329,7 @@
         <v>175</v>
       </c>
       <c r="B175">
-        <v>1023</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2337,7 +2337,7 @@
         <v>176</v>
       </c>
       <c r="B176">
-        <v>1023</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2345,7 +2345,7 @@
         <v>177</v>
       </c>
       <c r="B177">
-        <v>1023</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -2353,7 +2353,7 @@
         <v>178</v>
       </c>
       <c r="B178">
-        <v>1023</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2361,7 +2361,7 @@
         <v>179</v>
       </c>
       <c r="B179">
-        <v>1023</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2369,7 +2369,7 @@
         <v>180</v>
       </c>
       <c r="B180">
-        <v>1023</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2377,7 +2377,7 @@
         <v>181</v>
       </c>
       <c r="B181">
-        <v>1023</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2385,7 +2385,7 @@
         <v>182</v>
       </c>
       <c r="B182">
-        <v>1023</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -2393,7 +2393,7 @@
         <v>183</v>
       </c>
       <c r="B183">
-        <v>1158</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2401,7 +2401,7 @@
         <v>184</v>
       </c>
       <c r="B184">
-        <v>1158</v>
+        <v>1516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed error in calculating per capita gdp data
</commit_message>
<xml_diff>
--- a/NANCounts.xlsx
+++ b/NANCounts.xlsx
@@ -945,7 +945,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -953,7 +953,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -961,7 +961,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -969,7 +969,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -977,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -985,7 +985,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -993,7 +993,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1001,7 +1001,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1009,7 +1009,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1017,7 +1017,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1025,7 +1025,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1033,7 +1033,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1041,7 +1041,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1049,7 +1049,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1057,7 +1057,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1065,7 +1065,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1073,7 +1073,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1081,7 +1081,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1089,7 +1089,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1097,7 +1097,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1105,7 +1105,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1113,7 +1113,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1121,7 +1121,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1129,7 +1129,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1137,7 +1137,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1145,7 +1145,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1153,7 +1153,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1161,7 +1161,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1169,7 +1169,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1177,7 +1177,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1185,7 +1185,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1193,7 +1193,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1201,7 +1201,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1209,7 +1209,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1217,7 +1217,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1225,7 +1225,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1233,7 +1233,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1241,7 +1241,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1249,7 +1249,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1257,7 +1257,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1265,7 +1265,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1273,7 +1273,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1281,7 +1281,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1289,7 +1289,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1297,7 +1297,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1305,7 +1305,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1313,7 +1313,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1321,7 +1321,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1329,7 +1329,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1337,7 +1337,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1345,7 +1345,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1353,7 +1353,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1361,7 +1361,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1369,7 +1369,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1377,7 +1377,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1385,7 +1385,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1393,7 +1393,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1401,7 +1401,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1409,7 +1409,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1417,7 +1417,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1425,7 +1425,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1433,7 +1433,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1441,7 +1441,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1449,7 +1449,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1457,7 +1457,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1465,7 +1465,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1473,7 +1473,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1481,7 +1481,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1489,7 +1489,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1497,7 +1497,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1505,7 +1505,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1513,7 +1513,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1521,7 +1521,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1529,7 +1529,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1537,7 +1537,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1545,7 +1545,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1553,7 +1553,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1561,7 +1561,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1569,7 +1569,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1577,7 +1577,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1585,7 +1585,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1593,7 +1593,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1601,7 +1601,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1609,7 +1609,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1617,7 +1617,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1625,7 +1625,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1633,7 +1633,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1641,7 +1641,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1649,7 +1649,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>472</v>
+        <v>466</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1657,7 +1657,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1665,7 +1665,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1673,7 +1673,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1681,7 +1681,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1689,7 +1689,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1697,7 +1697,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>564</v>
+        <v>558</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1705,7 +1705,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>582</v>
+        <v>576</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1713,7 +1713,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1721,7 +1721,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1729,7 +1729,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1737,7 +1737,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1745,7 +1745,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1753,7 +1753,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1761,7 +1761,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1769,7 +1769,7 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1777,7 +1777,7 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1785,7 +1785,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1793,7 +1793,7 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1801,7 +1801,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1809,7 +1809,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1817,7 +1817,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1825,7 +1825,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1833,7 +1833,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1841,7 +1841,7 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1849,7 +1849,7 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1857,7 +1857,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1865,7 +1865,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1873,7 +1873,7 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1881,7 +1881,7 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1889,7 +1889,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1897,7 +1897,7 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>708</v>
+        <v>702</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1905,7 +1905,7 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>744</v>
+        <v>738</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1913,7 +1913,7 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>826</v>
+        <v>820</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1921,7 +1921,7 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>841</v>
+        <v>835</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1929,7 +1929,7 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>841</v>
+        <v>835</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1937,7 +1937,7 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>841</v>
+        <v>835</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1945,7 +1945,7 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>841</v>
+        <v>835</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1953,7 +1953,7 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>841</v>
+        <v>835</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1961,7 +1961,7 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>841</v>
+        <v>835</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1969,7 +1969,7 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>852</v>
+        <v>846</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1977,7 +1977,7 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>852</v>
+        <v>846</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1985,7 +1985,7 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>852</v>
+        <v>846</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1993,7 +1993,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>852</v>
+        <v>846</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2001,7 +2001,7 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>852</v>
+        <v>846</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2009,7 +2009,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>852</v>
+        <v>846</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2017,7 +2017,7 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>852</v>
+        <v>846</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2025,7 +2025,7 @@
         <v>137</v>
       </c>
       <c r="B137">
-        <v>852</v>
+        <v>846</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2033,7 +2033,7 @@
         <v>138</v>
       </c>
       <c r="B138">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2041,7 +2041,7 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2049,7 +2049,7 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2057,7 +2057,7 @@
         <v>141</v>
       </c>
       <c r="B141">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2065,7 +2065,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2073,7 +2073,7 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2081,7 +2081,7 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2089,7 +2089,7 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2097,7 +2097,7 @@
         <v>146</v>
       </c>
       <c r="B146">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2105,7 +2105,7 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2113,7 +2113,7 @@
         <v>148</v>
       </c>
       <c r="B148">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2121,7 +2121,7 @@
         <v>149</v>
       </c>
       <c r="B149">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2129,7 +2129,7 @@
         <v>150</v>
       </c>
       <c r="B150">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2137,7 +2137,7 @@
         <v>151</v>
       </c>
       <c r="B151">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2145,7 +2145,7 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2153,7 +2153,7 @@
         <v>153</v>
       </c>
       <c r="B153">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2161,7 +2161,7 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2169,7 +2169,7 @@
         <v>155</v>
       </c>
       <c r="B155">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2177,7 +2177,7 @@
         <v>156</v>
       </c>
       <c r="B156">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2185,7 +2185,7 @@
         <v>157</v>
       </c>
       <c r="B157">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2193,7 +2193,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2201,7 +2201,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2209,7 +2209,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2217,7 +2217,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2225,7 +2225,7 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2233,7 +2233,7 @@
         <v>163</v>
       </c>
       <c r="B163">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2241,7 +2241,7 @@
         <v>164</v>
       </c>
       <c r="B164">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2249,7 +2249,7 @@
         <v>165</v>
       </c>
       <c r="B165">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2257,7 +2257,7 @@
         <v>166</v>
       </c>
       <c r="B166">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2265,7 +2265,7 @@
         <v>167</v>
       </c>
       <c r="B167">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2273,7 +2273,7 @@
         <v>168</v>
       </c>
       <c r="B168">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -2281,7 +2281,7 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2289,7 +2289,7 @@
         <v>170</v>
       </c>
       <c r="B170">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2297,7 +2297,7 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2305,7 +2305,7 @@
         <v>172</v>
       </c>
       <c r="B172">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2313,7 +2313,7 @@
         <v>173</v>
       </c>
       <c r="B173">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2321,7 +2321,7 @@
         <v>174</v>
       </c>
       <c r="B174">
-        <v>1194</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2329,7 +2329,7 @@
         <v>175</v>
       </c>
       <c r="B175">
-        <v>1291</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2337,7 +2337,7 @@
         <v>176</v>
       </c>
       <c r="B176">
-        <v>1291</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2345,7 +2345,7 @@
         <v>177</v>
       </c>
       <c r="B177">
-        <v>1291</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -2353,7 +2353,7 @@
         <v>178</v>
       </c>
       <c r="B178">
-        <v>1291</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2361,7 +2361,7 @@
         <v>179</v>
       </c>
       <c r="B179">
-        <v>1291</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2369,7 +2369,7 @@
         <v>180</v>
       </c>
       <c r="B180">
-        <v>1291</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2377,7 +2377,7 @@
         <v>181</v>
       </c>
       <c r="B181">
-        <v>1291</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2385,7 +2385,7 @@
         <v>182</v>
       </c>
       <c r="B182">
-        <v>1291</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -2393,7 +2393,7 @@
         <v>183</v>
       </c>
       <c r="B183">
-        <v>1516</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2401,7 +2401,7 @@
         <v>184</v>
       </c>
       <c r="B184">
-        <v>1516</v>
+        <v>1510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>